<commit_message>
Updated a note at end of psa_yield_and_texture
I did NOT change the version, since no data entry changed. I just updated a note for demo purposes. will not deploy this version
</commit_message>
<xml_diff>
--- a/forms/psa_yield_and_texture/psa_yield_and_texture.xlsx
+++ b/forms/psa_yield_and_texture/psa_yield_and_texture.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saseehav\Documents\GitHub\Kobo\forms\psa_yield\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saseehav\Documents\GitHub\Kobo\forms\psa_yield_and_texture\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="5320"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -311,10 +311,10 @@
     <t>Welcome to the PSA form for Yield (for Corn, Cotton, or Soybean), that includes field hand harvest and taking soil texture. If you will remove sensors today also, please use the Sensor Uninstall Form as well</t>
   </si>
   <si>
-    <t>Return grain to lab, dry at low temperature if needed. Take moisture with moisture meter and weigh grain in a separate spreadsheet, found on the PSA Website. If you are removing sensors, please use the Kobo Form for Sensor unistalling</t>
-  </si>
-  <si>
     <t>row_spacing_inch</t>
+  </si>
+  <si>
+    <t>Return grain to lab, dry at low temperature if needed. Either dyr shelled grain to 0% or take moisture with moisture meter and weigh grain in a separate spreadsheet, found on the PSA Website. If you are removing sensors, please use the Kobo Form for Sensor unistalling</t>
   </si>
 </sst>
 </file>
@@ -658,14 +658,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.1796875" customWidth="1"/>
     <col min="2" max="2" width="19.453125" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
     <col min="5" max="5" width="22.90625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -806,7 +807,7 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C10" t="s">
         <v>27</v>
@@ -1339,7 +1340,7 @@
         <v>80</v>
       </c>
       <c r="C50" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F50" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Revert "Updated a note at end of psa_yield_and_texture"
This reverts commit dc512a7b0759dd17db61d94d04f23eb58742616b.
</commit_message>
<xml_diff>
--- a/forms/psa_yield_and_texture/psa_yield_and_texture.xlsx
+++ b/forms/psa_yield_and_texture/psa_yield_and_texture.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saseehav\Documents\GitHub\Kobo\forms\psa_yield_and_texture\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saseehav\Documents\GitHub\Kobo\forms\psa_yield\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="5320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -311,10 +311,10 @@
     <t>Welcome to the PSA form for Yield (for Corn, Cotton, or Soybean), that includes field hand harvest and taking soil texture. If you will remove sensors today also, please use the Sensor Uninstall Form as well</t>
   </si>
   <si>
+    <t>Return grain to lab, dry at low temperature if needed. Take moisture with moisture meter and weigh grain in a separate spreadsheet, found on the PSA Website. If you are removing sensors, please use the Kobo Form for Sensor unistalling</t>
+  </si>
+  <si>
     <t>row_spacing_inch</t>
-  </si>
-  <si>
-    <t>Return grain to lab, dry at low temperature if needed. Either dyr shelled grain to 0% or take moisture with moisture meter and weigh grain in a separate spreadsheet, found on the PSA Website. If you are removing sensors, please use the Kobo Form for Sensor unistalling</t>
   </si>
 </sst>
 </file>
@@ -658,15 +658,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.1796875" customWidth="1"/>
     <col min="2" max="2" width="19.453125" customWidth="1"/>
-    <col min="4" max="4" width="22" customWidth="1"/>
     <col min="5" max="5" width="22.90625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -807,7 +806,7 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C10" t="s">
         <v>27</v>
@@ -1340,7 +1339,7 @@
         <v>80</v>
       </c>
       <c r="C50" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F50" t="s">
         <v>13</v>

</xml_diff>